<commit_message>
App a funcionar antes de seleção de frequencia
</commit_message>
<xml_diff>
--- a/Estagio IAGO.xlsx
+++ b/Estagio IAGO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d6ecef277661d105/Ambiente de Trabalho/Work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d6ecef277661d105/Ambiente de Trabalho/Work/Estagio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{8BCAAD2C-7539-4C6A-965A-30436C611692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C8711F1-67A4-4006-83EA-6D035F0E0FFC}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{8BCAAD2C-7539-4C6A-965A-30436C611692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A735C31C-AD0A-45E8-8A40-BA8A9C22FA4D}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -201,9 +201,6 @@
     <t>Juros (€)</t>
   </si>
   <si>
-    <t>Contribuições (€)</t>
-  </si>
-  <si>
     <t>Saldo Final (€)</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>Meta</t>
+  </si>
+  <si>
+    <t>Reforço (€)</t>
   </si>
 </sst>
 </file>
@@ -220,11 +220,18 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -312,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -422,54 +429,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="9" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -503,71 +541,36 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -687,13 +690,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -711,6 +707,48 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -738,7 +776,7 @@
       <xdr:col>25</xdr:col>
       <xdr:colOff>20</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>109180</xdr:rowOff>
+      <xdr:rowOff>60334</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -775,18 +813,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A566140-A765-490C-8825-002CFD01B093}" name="Tabela1" displayName="Tabela1" ref="C2:H20" totalsRowShown="0" headerRowDxfId="2" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
-  <autoFilter ref="C2:H20" xr:uid="{3A566140-A765-490C-8825-002CFD01B093}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3A566140-A765-490C-8825-002CFD01B093}" name="Tabela1" displayName="Tabela1" ref="C2:H51" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
+  <autoFilter ref="C2:H51" xr:uid="{3A566140-A765-490C-8825-002CFD01B093}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2ABFFD89-6E6F-4247-8133-6C9927BFD049}" name="Ano" dataDxfId="6" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{1A3E28DE-9D07-4CE2-82C6-1291371BFAD4}" name="Saldo Inicial (€)" dataDxfId="5" dataCellStyle="Moeda"/>
-    <tableColumn id="6" xr3:uid="{9909D5E6-C020-47B2-B5B9-A9150E765811}" name="Taxa de juro (%)" dataDxfId="4" dataCellStyle="Percentagem"/>
-    <tableColumn id="3" xr3:uid="{10C2B428-002C-4A7E-A635-195EFD1310B5}" name="Juros (€)" dataDxfId="1" dataCellStyle="Moeda">
+    <tableColumn id="1" xr3:uid="{2ABFFD89-6E6F-4247-8133-6C9927BFD049}" name="Ano" dataDxfId="5" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{1A3E28DE-9D07-4CE2-82C6-1291371BFAD4}" name="Saldo Inicial (€)" dataDxfId="4" dataCellStyle="Moeda"/>
+    <tableColumn id="6" xr3:uid="{9909D5E6-C020-47B2-B5B9-A9150E765811}" name="Taxa de juro (%)" dataDxfId="3" dataCellStyle="Percentagem"/>
+    <tableColumn id="3" xr3:uid="{10C2B428-002C-4A7E-A635-195EFD1310B5}" name="Juros (€)" dataDxfId="2" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{2F9B4625-FDDB-47C9-9C66-B5B3C7B53A9E}" name="Contribuições (€)" dataDxfId="3" dataCellStyle="Moeda"/>
+    <tableColumn id="4" xr3:uid="{2F9B4625-FDDB-47C9-9C66-B5B3C7B53A9E}" name="Reforço (€)" dataDxfId="1" dataCellStyle="Moeda"/>
     <tableColumn id="5" xr3:uid="{A2A8B878-1644-433A-B220-5A0E49CBD1D8}" name="Saldo Final (€)" dataDxfId="0" dataCellStyle="Moeda">
-      <calculatedColumnFormula>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1000,18 +1038,18 @@
       <selection activeCell="D6" sqref="D6:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="113.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="12.5703125" style="1"/>
+    <col min="1" max="1" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="113.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="61.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="12.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1051,7 +1089,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1071,7 +1109,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1091,7 +1129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1111,7 +1149,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1131,7 +1169,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1151,7 +1189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1171,7 +1209,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1191,7 +1229,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1211,7 +1249,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1231,7 +1269,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1251,7 +1289,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1271,7 +1309,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1298,25 +1336,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E3B490D-FD75-47CC-B406-0A2D502A18C6}">
-  <dimension ref="B2:H20"/>
+  <dimension ref="B2:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="57" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="4" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.54296875" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" ht="14" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>52</v>
@@ -1325,404 +1363,1187 @@
         <v>53</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>54</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="2:8" ht="14" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
       </c>
       <c r="D3" s="10">
-        <v>500000</v>
+        <v>200000</v>
       </c>
       <c r="E3" s="11">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F3" s="12">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>50000</v>
+        <v>12000</v>
       </c>
       <c r="G3" s="10">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="H3" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v>560000</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>227000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="14" x14ac:dyDescent="0.25">
       <c r="C4" s="9">
         <f>IF(H3&gt;=$B$3,"",C3+1)</f>
         <v>2</v>
       </c>
       <c r="D4" s="12">
         <f>IF(H3&gt;=$B$3,"",H3)</f>
-        <v>560000</v>
+        <v>227000</v>
       </c>
       <c r="E4" s="11">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F4" s="12">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>56000</v>
+        <v>13620</v>
       </c>
       <c r="G4" s="10">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="H4" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v>626000</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>255620</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="14" x14ac:dyDescent="0.25">
       <c r="C5" s="9">
-        <f t="shared" ref="C5:C20" si="0">IF(H4&gt;=$B$3,"",C4+1)</f>
+        <f t="shared" ref="C5:C19" si="0">IF(H4&gt;=$B$3,"",C4+1)</f>
         <v>3</v>
       </c>
       <c r="D5" s="12">
-        <f t="shared" ref="D5:D20" si="1">IF(H4&gt;=$B$3,"",H4)</f>
-        <v>626000</v>
+        <f t="shared" ref="D5:D19" si="1">IF(H4&gt;=$B$3,"",H4)</f>
+        <v>255620</v>
       </c>
       <c r="E5" s="11">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F5" s="12">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>62600</v>
+        <v>15337.199999999999</v>
       </c>
       <c r="G5" s="10">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="H5" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v>698600</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>285957.2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="14" x14ac:dyDescent="0.25">
       <c r="C6" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="1"/>
-        <v>698600</v>
+        <v>285957.2</v>
       </c>
       <c r="E6" s="11">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F6" s="12">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>69860</v>
+        <v>17157.432000000001</v>
       </c>
       <c r="G6" s="10">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="H6" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v>778460</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>318114.63199999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="14" x14ac:dyDescent="0.25">
       <c r="C7" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D7" s="12">
         <f t="shared" si="1"/>
-        <v>778460</v>
+        <v>318114.63199999998</v>
       </c>
       <c r="E7" s="11">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F7" s="12">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>77846</v>
+        <v>19086.877919999999</v>
       </c>
       <c r="G7" s="10">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="H7" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v>866306</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>352201.50991999998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="14" x14ac:dyDescent="0.25">
       <c r="C8" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D8" s="12">
         <f t="shared" si="1"/>
-        <v>866306</v>
+        <v>352201.50991999998</v>
       </c>
       <c r="E8" s="11">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F8" s="12">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>86630.6</v>
+        <v>21132.090595199999</v>
       </c>
       <c r="G8" s="10">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="H8" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v>962936.6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>388333.6005152</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="14" x14ac:dyDescent="0.25">
       <c r="C9" s="9">
         <f>IF(H8&gt;=$B$3,"",C8+1)</f>
         <v>7</v>
       </c>
       <c r="D9" s="12">
         <f t="shared" si="1"/>
-        <v>962936.6</v>
+        <v>388333.6005152</v>
       </c>
       <c r="E9" s="11">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F9" s="12">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>96293.66</v>
+        <v>23300.016030912</v>
       </c>
       <c r="G9" s="10">
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="H9" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v>1069230.26</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C10" s="9" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>426633.616546112</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C10" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D10" s="12" t="str">
+        <v>8</v>
+      </c>
+      <c r="D10" s="12">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="14" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C11" s="9" t="str">
+        <v>426633.616546112</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F10" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>25598.016992766719</v>
+      </c>
+      <c r="G10" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H10" s="14">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>467231.6335388787</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C11" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D11" s="12" t="str">
+        <v>9</v>
+      </c>
+      <c r="D11" s="12">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="14" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C12" s="9" t="str">
+        <v>467231.6335388787</v>
+      </c>
+      <c r="E11" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F11" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>28033.89801233272</v>
+      </c>
+      <c r="G11" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H11" s="14">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>510265.53155121143</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C12" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D12" s="12" t="str">
+        <v>10</v>
+      </c>
+      <c r="D12" s="12">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="14" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C13" s="9" t="str">
+        <v>510265.53155121143</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F12" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>30615.931893072684</v>
+      </c>
+      <c r="G12" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H12" s="14">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>555881.46344428416</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C13" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D13" s="12" t="str">
+        <v>11</v>
+      </c>
+      <c r="D13" s="12">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="14" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C14" s="9" t="str">
+        <v>555881.46344428416</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F13" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>33352.887806657047</v>
+      </c>
+      <c r="G13" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H13" s="14">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>604234.35125094117</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C14" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D14" s="12" t="str">
+        <v>12</v>
+      </c>
+      <c r="D14" s="12">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="14" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C15" s="9" t="str">
+        <v>604234.35125094117</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F14" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>36254.061075056467</v>
+      </c>
+      <c r="G14" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H14" s="14">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>655488.4123259976</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C15" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D15" s="12" t="str">
+        <v>13</v>
+      </c>
+      <c r="D15" s="12">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="14" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C16" s="9" t="str">
+        <v>655488.4123259976</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F15" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>39329.304739559855</v>
+      </c>
+      <c r="G15" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H15" s="14">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>709817.71706555749</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C16" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D16" s="12" t="str">
+        <v>14</v>
+      </c>
+      <c r="D16" s="12">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="14" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C17" s="9" t="str">
+        <v>709817.71706555749</v>
+      </c>
+      <c r="E16" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F16" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>42589.06302393345</v>
+      </c>
+      <c r="G16" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H16" s="14">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>767406.78008949093</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C17" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D17" s="12" t="str">
+        <v>15</v>
+      </c>
+      <c r="D17" s="12">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="14" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C18" s="9" t="str">
+        <v>767406.78008949093</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F17" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>46044.406805369457</v>
+      </c>
+      <c r="G17" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H17" s="14">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>828451.18689486035</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C18" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D18" s="12" t="str">
+        <v>16</v>
+      </c>
+      <c r="D18" s="12">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="14" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C19" s="9" t="str">
+        <v>828451.18689486035</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F18" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>49707.071213691619</v>
+      </c>
+      <c r="G18" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H18" s="14">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>893158.25810855196</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C19" s="9">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D19" s="12" t="str">
+        <v>17</v>
+      </c>
+      <c r="D19" s="12">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="14" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C20" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D20" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v/>
-      </c>
-      <c r="G20" s="10"/>
-      <c r="H20" s="15" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Contribuições (€)]])</f>
+        <v>893158.25810855196</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F19" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>53589.495486513115</v>
+      </c>
+      <c r="G19" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H19" s="14">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>961747.75359506509</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C20" s="9">
+        <f>IF(H19&gt;=$B$3,"",C19+1)</f>
+        <v>18</v>
+      </c>
+      <c r="D20" s="12">
+        <f>IF(H19&gt;=$B$3,"",H19)</f>
+        <v>961747.75359506509</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F20" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>57704.865215703903</v>
+      </c>
+      <c r="G20" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H20" s="15">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>1034452.6188107689</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C21" s="9">
+        <f t="shared" ref="C21:C50" si="2">IF(H20&gt;=$B$3,"",C20+1)</f>
+        <v>19</v>
+      </c>
+      <c r="D21" s="12">
+        <f t="shared" ref="D21:D51" si="3">IF(H20&gt;=$B$3,"",H20)</f>
+        <v>1034452.6188107689</v>
+      </c>
+      <c r="E21" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F21" s="18">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>62067.157128646133</v>
+      </c>
+      <c r="G21" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H21" s="19">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>1111519.775939415</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C22" s="9">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="D22" s="12">
+        <f t="shared" si="3"/>
+        <v>1111519.775939415</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F22" s="18">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>66691.18655636489</v>
+      </c>
+      <c r="G22" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H22" s="19">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>1193210.9624957799</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C23" s="9">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D23" s="12">
+        <f t="shared" si="3"/>
+        <v>1193210.9624957799</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F23" s="18">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>71592.657749746795</v>
+      </c>
+      <c r="G23" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H23" s="19">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>1279803.6202455265</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C24" s="9">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D24" s="12">
+        <f t="shared" si="3"/>
+        <v>1279803.6202455265</v>
+      </c>
+      <c r="E24" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F24" s="18">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>76788.217214731587</v>
+      </c>
+      <c r="G24" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H24" s="19">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>1371591.837460258</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C25" s="9">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="D25" s="12">
+        <f t="shared" si="3"/>
+        <v>1371591.837460258</v>
+      </c>
+      <c r="E25" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F25" s="18">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>82295.510247615486</v>
+      </c>
+      <c r="G25" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H25" s="19">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>1468887.3477078734</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C26" s="9">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D26" s="12">
+        <f t="shared" si="3"/>
+        <v>1468887.3477078734</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F26" s="18">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>88133.240862472405</v>
+      </c>
+      <c r="G26" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H26" s="19">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>1572020.5885703459</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C27" s="9">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="D27" s="12">
+        <f t="shared" si="3"/>
+        <v>1572020.5885703459</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F27" s="18">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>94321.235314220743</v>
+      </c>
+      <c r="G27" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H27" s="19">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>1681341.8238845665</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C28" s="9">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="D28" s="12">
+        <f t="shared" si="3"/>
+        <v>1681341.8238845665</v>
+      </c>
+      <c r="E28" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F28" s="18">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>100880.509433074</v>
+      </c>
+      <c r="G28" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H28" s="19">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>1797222.3333176405</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C29" s="9">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="D29" s="12">
+        <f t="shared" si="3"/>
+        <v>1797222.3333176405</v>
+      </c>
+      <c r="E29" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F29" s="18">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>107833.33999905843</v>
+      </c>
+      <c r="G29" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H29" s="19">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>1920055.673316699</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C30" s="9">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="D30" s="12">
+        <f t="shared" si="3"/>
+        <v>1920055.673316699</v>
+      </c>
+      <c r="E30" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F30" s="18">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>115203.34039900193</v>
+      </c>
+      <c r="G30" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H30" s="19">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>2050259.0137157009</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C31" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D31" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E31" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F31" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G31" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H31" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C32" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D32" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E32" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F32" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G32" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H32" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C33" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D33" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E33" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F33" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G33" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H33" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C34" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D34" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E34" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F34" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G34" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H34" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C35" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D35" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E35" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F35" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G35" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H35" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C36" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D36" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E36" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F36" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G36" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H36" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C37" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D37" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E37" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F37" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G37" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H37" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C38" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D38" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E38" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F38" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G38" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H38" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C39" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D39" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E39" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F39" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G39" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H39" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C40" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D40" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E40" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F40" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G40" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H40" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C41" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D41" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E41" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F41" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G41" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H41" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C42" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D42" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E42" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F42" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G42" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H42" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C43" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D43" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E43" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F43" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G43" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H43" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C44" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D44" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E44" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F44" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G44" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H44" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C45" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D45" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E45" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F45" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G45" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H45" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C46" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D46" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E46" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F46" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G46" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H46" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C47" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D47" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E47" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F47" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G47" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H47" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C48" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D48" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E48" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F48" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G48" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H48" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C49" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D49" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E49" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F49" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G49" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H49" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C50" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D50" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E50" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F50" s="20" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G50" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H50" s="21" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+      <c r="C51" s="16"/>
+      <c r="D51" s="12" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E51" s="17"/>
+      <c r="F51" s="18" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
+      </c>
+      <c r="G51" s="10">
+        <v>15000</v>
+      </c>
+      <c r="H51" s="19" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Update investment calculator app and Excel file
</commit_message>
<xml_diff>
--- a/Estagio IAGO.xlsx
+++ b/Estagio IAGO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d6ecef277661d105/Ambiente de Trabalho/Work/Estagio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{8BCAAD2C-7539-4C6A-965A-30436C611692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A735C31C-AD0A-45E8-8A40-BA8A9C22FA4D}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{8BCAAD2C-7539-4C6A-965A-30436C611692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F02B0CF6-F9D8-483F-A2D5-B737B4198A1E}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -477,9 +477,6 @@
     <xf numFmtId="44" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -492,22 +489,16 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -518,81 +509,6 @@
     <cellStyle name="Percentagem" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -610,6 +526,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -617,13 +534,64 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -639,6 +607,12 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -817,13 +791,13 @@
   <autoFilter ref="C2:H51" xr:uid="{3A566140-A765-490C-8825-002CFD01B093}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{2ABFFD89-6E6F-4247-8133-6C9927BFD049}" name="Ano" dataDxfId="5" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{1A3E28DE-9D07-4CE2-82C6-1291371BFAD4}" name="Saldo Inicial (€)" dataDxfId="4" dataCellStyle="Moeda"/>
-    <tableColumn id="6" xr3:uid="{9909D5E6-C020-47B2-B5B9-A9150E765811}" name="Taxa de juro (%)" dataDxfId="3" dataCellStyle="Percentagem"/>
-    <tableColumn id="3" xr3:uid="{10C2B428-002C-4A7E-A635-195EFD1310B5}" name="Juros (€)" dataDxfId="2" dataCellStyle="Moeda">
+    <tableColumn id="2" xr3:uid="{1A3E28DE-9D07-4CE2-82C6-1291371BFAD4}" name="Saldo Inicial (€)" dataDxfId="2" dataCellStyle="Moeda"/>
+    <tableColumn id="6" xr3:uid="{9909D5E6-C020-47B2-B5B9-A9150E765811}" name="Taxa de juro (%)" dataDxfId="0" dataCellStyle="Percentagem"/>
+    <tableColumn id="3" xr3:uid="{10C2B428-002C-4A7E-A635-195EFD1310B5}" name="Juros (€)" dataDxfId="1" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{2F9B4625-FDDB-47C9-9C66-B5B3C7B53A9E}" name="Reforço (€)" dataDxfId="1" dataCellStyle="Moeda"/>
-    <tableColumn id="5" xr3:uid="{A2A8B878-1644-433A-B220-5A0E49CBD1D8}" name="Saldo Final (€)" dataDxfId="0" dataCellStyle="Moeda">
+    <tableColumn id="4" xr3:uid="{2F9B4625-FDDB-47C9-9C66-B5B3C7B53A9E}" name="Reforço (€)" dataDxfId="4" dataCellStyle="Moeda"/>
+    <tableColumn id="5" xr3:uid="{A2A8B878-1644-433A-B220-5A0E49CBD1D8}" name="Saldo Final (€)" dataDxfId="3" dataCellStyle="Moeda">
       <calculatedColumnFormula>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1035,21 +1009,21 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D5" sqref="D5:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="113.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="12.54296875" style="1"/>
+    <col min="1" max="1" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="124" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.28515625" style="1" customWidth="1"/>
+    <col min="7" max="12" width="12.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1069,7 +1043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1089,7 +1063,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1109,7 +1083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1129,7 +1103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1149,7 +1123,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1169,7 +1143,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1189,7 +1163,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1209,7 +1183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1229,7 +1203,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1249,7 +1223,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1269,7 +1243,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1289,7 +1263,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1309,7 +1283,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1339,20 +1313,20 @@
   <dimension ref="B2:H51"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+      <selection activeCell="E3" sqref="E3:E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="5" width="18.453125" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.54296875" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="4" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>57</v>
       </c>
@@ -1375,1174 +1349,1174 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B3" s="6">
-        <v>2000000</v>
+        <v>200000</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
       </c>
       <c r="D3" s="10">
-        <v>200000</v>
-      </c>
-      <c r="E3" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F3" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>12000</v>
+        <v>50000</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="11">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>2500</v>
       </c>
       <c r="G3" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H3" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>227000</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>62500</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C4" s="9">
         <f>IF(H3&gt;=$B$3,"",C3+1)</f>
         <v>2</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <f>IF(H3&gt;=$B$3,"",H3)</f>
-        <v>227000</v>
-      </c>
-      <c r="E4" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F4" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>13620</v>
+        <v>62500</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F4" s="11">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>3125</v>
       </c>
       <c r="G4" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H4" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>255620</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>75625</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C5" s="9">
         <f t="shared" ref="C5:C19" si="0">IF(H4&gt;=$B$3,"",C4+1)</f>
         <v>3</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <f t="shared" ref="D5:D19" si="1">IF(H4&gt;=$B$3,"",H4)</f>
-        <v>255620</v>
-      </c>
-      <c r="E5" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F5" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>15337.199999999999</v>
+        <v>75625</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="11">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>3781.25</v>
       </c>
       <c r="G5" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H5" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>285957.2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H5" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>89406.25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C6" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <f t="shared" si="1"/>
-        <v>285957.2</v>
-      </c>
-      <c r="E6" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F6" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>17157.432000000001</v>
+        <v>89406.25</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F6" s="11">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>4470.3125</v>
       </c>
       <c r="G6" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H6" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>318114.63199999998</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H6" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>103876.5625</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C7" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <f t="shared" si="1"/>
-        <v>318114.63199999998</v>
-      </c>
-      <c r="E7" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F7" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>19086.877919999999</v>
+        <v>103876.5625</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="11">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>5193.828125</v>
       </c>
       <c r="G7" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H7" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>352201.50991999998</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H7" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>119070.390625</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C8" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <f t="shared" si="1"/>
-        <v>352201.50991999998</v>
-      </c>
-      <c r="E8" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F8" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>21132.090595199999</v>
+        <v>119070.390625</v>
+      </c>
+      <c r="E8" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F8" s="11">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>5953.51953125</v>
       </c>
       <c r="G8" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H8" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>388333.6005152</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H8" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>135023.91015625</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C9" s="9">
         <f>IF(H8&gt;=$B$3,"",C8+1)</f>
         <v>7</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <f t="shared" si="1"/>
-        <v>388333.6005152</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F9" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>23300.016030912</v>
+        <v>135023.91015625</v>
+      </c>
+      <c r="E9" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="11">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>6751.1955078125002</v>
       </c>
       <c r="G9" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H9" s="13">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>426633.616546112</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H9" s="12">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>151775.10566406249</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C10" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <f t="shared" si="1"/>
-        <v>426633.616546112</v>
-      </c>
-      <c r="E10" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F10" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>25598.016992766719</v>
+        <v>151775.10566406249</v>
+      </c>
+      <c r="E10" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F10" s="11">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>7588.7552832031251</v>
       </c>
       <c r="G10" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H10" s="14">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>467231.6335388787</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H10" s="13">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>169363.86094726561</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C11" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <f t="shared" si="1"/>
-        <v>467231.6335388787</v>
-      </c>
-      <c r="E11" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F11" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>28033.89801233272</v>
+        <v>169363.86094726561</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="11">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>8468.1930473632801</v>
       </c>
       <c r="G11" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H11" s="14">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>510265.53155121143</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H11" s="13">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>187832.05399462889</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C12" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <f t="shared" si="1"/>
-        <v>510265.53155121143</v>
-      </c>
-      <c r="E12" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F12" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>30615.931893072684</v>
+        <v>187832.05399462889</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F12" s="11">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v>9391.6026997314457</v>
       </c>
       <c r="G12" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H12" s="14">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>555881.46344428416</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C13" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H12" s="13">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v>207223.65669436034</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C13" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="D13" s="12">
+        <v/>
+      </c>
+      <c r="D13" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>555881.46344428416</v>
-      </c>
-      <c r="E13" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F13" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>33352.887806657047</v>
+        <v/>
+      </c>
+      <c r="E13" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F13" s="11" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G13" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H13" s="14">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>604234.35125094117</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C14" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H13" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C14" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="D14" s="12">
+        <v/>
+      </c>
+      <c r="D14" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>604234.35125094117</v>
-      </c>
-      <c r="E14" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F14" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>36254.061075056467</v>
+        <v/>
+      </c>
+      <c r="E14" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F14" s="11" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G14" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H14" s="14">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>655488.4123259976</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C15" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H14" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C15" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="D15" s="12">
+        <v/>
+      </c>
+      <c r="D15" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>655488.4123259976</v>
-      </c>
-      <c r="E15" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F15" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>39329.304739559855</v>
+        <v/>
+      </c>
+      <c r="E15" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="11" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G15" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H15" s="14">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>709817.71706555749</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C16" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H15" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C16" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="D16" s="12">
+        <v/>
+      </c>
+      <c r="D16" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>709817.71706555749</v>
-      </c>
-      <c r="E16" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F16" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>42589.06302393345</v>
+        <v/>
+      </c>
+      <c r="E16" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F16" s="11" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G16" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H16" s="14">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>767406.78008949093</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C17" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H16" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C17" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="D17" s="12">
+        <v/>
+      </c>
+      <c r="D17" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>767406.78008949093</v>
-      </c>
-      <c r="E17" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F17" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>46044.406805369457</v>
+        <v/>
+      </c>
+      <c r="E17" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F17" s="11" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G17" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H17" s="14">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>828451.18689486035</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C18" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H17" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C18" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="D18" s="12">
+        <v/>
+      </c>
+      <c r="D18" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>828451.18689486035</v>
-      </c>
-      <c r="E18" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F18" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>49707.071213691619</v>
+        <v/>
+      </c>
+      <c r="E18" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F18" s="11" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G18" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H18" s="14">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>893158.25810855196</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C19" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H18" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C19" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="D19" s="12">
+        <v/>
+      </c>
+      <c r="D19" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>893158.25810855196</v>
-      </c>
-      <c r="E19" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F19" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>53589.495486513115</v>
+        <v/>
+      </c>
+      <c r="E19" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F19" s="11" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G19" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H19" s="14">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>961747.75359506509</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C20" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H19" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C20" s="9" t="str">
         <f>IF(H19&gt;=$B$3,"",C19+1)</f>
-        <v>18</v>
-      </c>
-      <c r="D20" s="12">
+        <v/>
+      </c>
+      <c r="D20" s="11" t="str">
         <f>IF(H19&gt;=$B$3,"",H19)</f>
-        <v>961747.75359506509</v>
-      </c>
-      <c r="E20" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F20" s="12">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>57704.865215703903</v>
+        <v/>
+      </c>
+      <c r="E20" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F20" s="11" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G20" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H20" s="15">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>1034452.6188107689</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C21" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H20" s="14" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C21" s="9" t="str">
         <f t="shared" ref="C21:C50" si="2">IF(H20&gt;=$B$3,"",C20+1)</f>
-        <v>19</v>
-      </c>
-      <c r="D21" s="12">
+        <v/>
+      </c>
+      <c r="D21" s="11" t="str">
         <f t="shared" ref="D21:D51" si="3">IF(H20&gt;=$B$3,"",H20)</f>
-        <v>1034452.6188107689</v>
-      </c>
-      <c r="E21" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F21" s="18">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>62067.157128646133</v>
+        <v/>
+      </c>
+      <c r="E21" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F21" s="15" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G21" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H21" s="19">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>1111519.775939415</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C22" s="9">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="D22" s="12">
-        <f t="shared" si="3"/>
-        <v>1111519.775939415</v>
-      </c>
-      <c r="E22" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F22" s="18">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>66691.18655636489</v>
+        <v>10000</v>
+      </c>
+      <c r="H21" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C22" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D22" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E22" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F22" s="15" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G22" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H22" s="19">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>1193210.9624957799</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C23" s="9">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="D23" s="12">
-        <f t="shared" si="3"/>
-        <v>1193210.9624957799</v>
-      </c>
-      <c r="E23" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F23" s="18">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>71592.657749746795</v>
+        <v>10000</v>
+      </c>
+      <c r="H22" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C23" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D23" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E23" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F23" s="15" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G23" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H23" s="19">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>1279803.6202455265</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C24" s="9">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="D24" s="12">
-        <f t="shared" si="3"/>
-        <v>1279803.6202455265</v>
-      </c>
-      <c r="E24" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F24" s="18">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>76788.217214731587</v>
+        <v>10000</v>
+      </c>
+      <c r="H23" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C24" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D24" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E24" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F24" s="15" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G24" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H24" s="19">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>1371591.837460258</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C25" s="9">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="D25" s="12">
-        <f t="shared" si="3"/>
-        <v>1371591.837460258</v>
-      </c>
-      <c r="E25" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F25" s="18">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>82295.510247615486</v>
+        <v>10000</v>
+      </c>
+      <c r="H24" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C25" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D25" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E25" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F25" s="15" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G25" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H25" s="19">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>1468887.3477078734</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C26" s="9">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="D26" s="12">
-        <f t="shared" si="3"/>
-        <v>1468887.3477078734</v>
-      </c>
-      <c r="E26" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F26" s="18">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>88133.240862472405</v>
+        <v>10000</v>
+      </c>
+      <c r="H25" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C26" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D26" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E26" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F26" s="15" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G26" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H26" s="19">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>1572020.5885703459</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C27" s="9">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="D27" s="12">
-        <f t="shared" si="3"/>
-        <v>1572020.5885703459</v>
-      </c>
-      <c r="E27" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F27" s="18">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>94321.235314220743</v>
+        <v>10000</v>
+      </c>
+      <c r="H26" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C27" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D27" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E27" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F27" s="15" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G27" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H27" s="19">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>1681341.8238845665</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C28" s="9">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="D28" s="12">
-        <f t="shared" si="3"/>
-        <v>1681341.8238845665</v>
-      </c>
-      <c r="E28" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F28" s="18">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>100880.509433074</v>
+        <v>10000</v>
+      </c>
+      <c r="H27" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C28" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D28" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E28" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F28" s="15" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G28" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H28" s="19">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>1797222.3333176405</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C29" s="9">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="D29" s="12">
-        <f t="shared" si="3"/>
-        <v>1797222.3333176405</v>
-      </c>
-      <c r="E29" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F29" s="18">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>107833.33999905843</v>
+        <v>10000</v>
+      </c>
+      <c r="H28" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C29" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D29" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E29" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F29" s="15" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G29" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H29" s="19">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>1920055.673316699</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C30" s="9">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="D30" s="12">
-        <f t="shared" si="3"/>
-        <v>1920055.673316699</v>
-      </c>
-      <c r="E30" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F30" s="18">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
-        <v>115203.34039900193</v>
+        <v>10000</v>
+      </c>
+      <c r="H29" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C30" s="9" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="D30" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E30" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F30" s="15" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
+        <v/>
       </c>
       <c r="G30" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H30" s="19">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v>2050259.0137157009</v>
-      </c>
-    </row>
-    <row r="31" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H30" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C31" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D31" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E31" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F31" s="18" t="str">
+      <c r="D31" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E31" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F31" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G31" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H31" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H31" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C32" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D32" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E32" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F32" s="18" t="str">
+      <c r="D32" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E32" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F32" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G32" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H32" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H32" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C33" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D33" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E33" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F33" s="18" t="str">
+      <c r="D33" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E33" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F33" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G33" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H33" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H33" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C34" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D34" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E34" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F34" s="18" t="str">
+      <c r="D34" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E34" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F34" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G34" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H34" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H34" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C35" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D35" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E35" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F35" s="18" t="str">
+      <c r="D35" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E35" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F35" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G35" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H35" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H35" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C36" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D36" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E36" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F36" s="18" t="str">
+      <c r="D36" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E36" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F36" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G36" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H36" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H36" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C37" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D37" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E37" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F37" s="18" t="str">
+      <c r="D37" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E37" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F37" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G37" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H37" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H37" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C38" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D38" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E38" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F38" s="18" t="str">
+      <c r="D38" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E38" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F38" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G38" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H38" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H38" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C39" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D39" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E39" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F39" s="18" t="str">
+      <c r="D39" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E39" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F39" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G39" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H39" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H39" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C40" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D40" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E40" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F40" s="18" t="str">
+      <c r="D40" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E40" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F40" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G40" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H40" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H40" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C41" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D41" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E41" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F41" s="18" t="str">
+      <c r="D41" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E41" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F41" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G41" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H41" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H41" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C42" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D42" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E42" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F42" s="18" t="str">
+      <c r="D42" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E42" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F42" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G42" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H42" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H42" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C43" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D43" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E43" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F43" s="18" t="str">
+      <c r="D43" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E43" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F43" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G43" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H43" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H43" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C44" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D44" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E44" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F44" s="18" t="str">
+      <c r="D44" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E44" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F44" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G44" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H44" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H44" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C45" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D45" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E45" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F45" s="18" t="str">
+      <c r="D45" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E45" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F45" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G45" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H45" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H45" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C46" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D46" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E46" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F46" s="18" t="str">
+      <c r="D46" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E46" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F46" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G46" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H46" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H46" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C47" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D47" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E47" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F47" s="18" t="str">
+      <c r="D47" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E47" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F47" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G47" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H47" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H47" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C48" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D48" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E48" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F48" s="18" t="str">
+      <c r="D48" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E48" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F48" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G48" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H48" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H48" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C49" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D49" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E49" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F49" s="18" t="str">
+      <c r="D49" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E49" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F49" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G49" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H49" s="19" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="3:8" ht="14" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="H49" s="13" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C50" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D50" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E50" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F50" s="20" t="str">
+      <c r="D50" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E50" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="F50" s="16" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G50" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H50" s="21" t="str">
-        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="3:8" ht="14" x14ac:dyDescent="0.25">
-      <c r="C51" s="16"/>
-      <c r="D51" s="12" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E51" s="17"/>
-      <c r="F51" s="18" t="str">
+        <v>10000</v>
+      </c>
+      <c r="H50" s="14" t="str">
+        <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="3:8" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C51" s="9"/>
+      <c r="D51" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E51" s="18"/>
+      <c r="F51" s="15" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]*Tabela1[[#This Row],[Taxa de juro (%)]])</f>
         <v/>
       </c>
       <c r="G51" s="10">
-        <v>15000</v>
-      </c>
-      <c r="H51" s="19" t="str">
+        <v>10000</v>
+      </c>
+      <c r="H51" s="13" t="str">
         <f>IF(Tabela1[[#This Row],[Ano]]="","",Tabela1[[#This Row],[Saldo Inicial (€)]]+Tabela1[[#This Row],[Juros (€)]]+Tabela1[[#This Row],[Reforço (€)]])</f>
         <v/>
       </c>

</xml_diff>